<commit_message>
EOS as shadow kernel, joystick support
</commit_message>
<xml_diff>
--- a/measurements.xlsx
+++ b/measurements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mario/Development/AgonLight/software/AgonElectronOS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73888B15-4AF1-694C-868F-B7A017E575D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E5AC74F-1082-D848-96E5-69B9AC4DA90F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="1060" windowWidth="29720" windowHeight="17820" xr2:uid="{ECD59F6F-C4A5-C740-9F2E-095C6D77DE08}"/>
+    <workbookView xWindow="0" yWindow="940" windowWidth="29720" windowHeight="17820" activeTab="1" xr2:uid="{ECD59F6F-C4A5-C740-9F2E-095C6D77DE08}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -719,7 +719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47D49604-FCB0-4E48-8419-D053DBDD9CC9}">
   <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
@@ -1574,7 +1574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5B66013-96C2-0146-9E53-8F74B0183863}">
   <dimension ref="A1:BB21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>

</xml_diff>